<commit_message>
burn up/down - oppdatert t.o.m. 7/3/14
</commit_message>
<xml_diff>
--- a/Sprint 4/SysUt14 Gr 2 Burn down chart - holdes oppdatert av SM.xlsx
+++ b/Sprint 4/SysUt14 Gr 2 Burn down chart - holdes oppdatert av SM.xlsx
@@ -635,31 +635,31 @@
                   <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>147</c:v>
+                  <c:v>125.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51578368"/>
-        <c:axId val="51579904"/>
+        <c:axId val="51458432"/>
+        <c:axId val="51459968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51578368"/>
+        <c:axId val="51458432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51579904"/>
+        <c:crossAx val="51459968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51579904"/>
+        <c:axId val="51459968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -669,7 +669,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51578368"/>
+        <c:crossAx val="51458432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1066,7 +1066,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1208,7 +1208,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
@@ -1250,7 +1250,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
@@ -1332,7 +1332,7 @@
         <v>3</v>
       </c>
       <c r="K6" s="8">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="L6" s="22"/>
       <c r="M6" s="22"/>
@@ -1740,7 +1740,7 @@
         <v>18</v>
       </c>
       <c r="K16" s="7">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
@@ -1822,7 +1822,7 @@
         <v>18.5</v>
       </c>
       <c r="K18" s="7">
-        <v>18.5</v>
+        <v>14.5</v>
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
@@ -1864,7 +1864,7 @@
         <v>37</v>
       </c>
       <c r="K19" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -1948,7 +1948,7 @@
         <v>15</v>
       </c>
       <c r="K21" s="7">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="K23" s="16">
         <f t="shared" si="0"/>
-        <v>147</v>
+        <v>125.5</v>
       </c>
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>

</xml_diff>

<commit_message>
Redigerte en feil i ukedagene
</commit_message>
<xml_diff>
--- a/Sprint 4/SysUt14 Gr 2 Burn down chart - holdes oppdatert av SM.xlsx
+++ b/Sprint 4/SysUt14 Gr 2 Burn down chart - holdes oppdatert av SM.xlsx
@@ -635,6 +635,9 @@
                   <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>125.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -642,24 +645,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51458432"/>
-        <c:axId val="51459968"/>
+        <c:axId val="50810240"/>
+        <c:axId val="51518464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51458432"/>
+        <c:axId val="50810240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51459968"/>
+        <c:crossAx val="51518464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51459968"/>
+        <c:axId val="51518464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -669,7 +672,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51458432"/>
+        <c:crossAx val="50810240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1065,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1168,7 +1171,9 @@
       <c r="K2" s="7">
         <v>0</v>
       </c>
-      <c r="L2" s="7"/>
+      <c r="L2" s="7">
+        <v>0</v>
+      </c>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
@@ -1208,9 +1213,11 @@
         <v>2</v>
       </c>
       <c r="K3" s="7">
-        <v>0</v>
-      </c>
-      <c r="L3" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
@@ -1250,9 +1257,11 @@
         <v>2</v>
       </c>
       <c r="K4" s="8">
-        <v>0</v>
-      </c>
-      <c r="L4" s="22"/>
+        <v>2</v>
+      </c>
+      <c r="L4" s="8">
+        <v>0</v>
+      </c>
       <c r="M4" s="22"/>
       <c r="N4" s="8"/>
       <c r="O4" s="7"/>
@@ -1294,7 +1303,9 @@
       <c r="K5" s="8">
         <v>1.5</v>
       </c>
-      <c r="L5" s="22"/>
+      <c r="L5" s="8">
+        <v>1.5</v>
+      </c>
       <c r="M5" s="22"/>
       <c r="N5" s="8"/>
       <c r="O5" s="7"/>
@@ -1332,9 +1343,11 @@
         <v>3</v>
       </c>
       <c r="K6" s="8">
+        <v>3</v>
+      </c>
+      <c r="L6" s="8">
         <v>0.5</v>
       </c>
-      <c r="L6" s="22"/>
       <c r="M6" s="22"/>
       <c r="N6" s="8"/>
       <c r="O6" s="7"/>
@@ -1374,7 +1387,9 @@
       <c r="K7" s="8">
         <v>1</v>
       </c>
-      <c r="L7" s="8"/>
+      <c r="L7" s="8">
+        <v>1</v>
+      </c>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="7"/>
@@ -1416,7 +1431,9 @@
       <c r="K8" s="8">
         <v>10</v>
       </c>
-      <c r="L8" s="8"/>
+      <c r="L8" s="8">
+        <v>10</v>
+      </c>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="7"/>
@@ -1456,7 +1473,9 @@
       <c r="K9" s="8">
         <v>0</v>
       </c>
-      <c r="L9" s="8"/>
+      <c r="L9" s="8">
+        <v>0</v>
+      </c>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="7"/>
@@ -1498,7 +1517,9 @@
       <c r="K10" s="7">
         <v>0</v>
       </c>
-      <c r="L10" s="8"/>
+      <c r="L10" s="7">
+        <v>0</v>
+      </c>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="7"/>
@@ -1538,7 +1559,9 @@
       <c r="K11" s="7">
         <v>0</v>
       </c>
-      <c r="L11" s="8"/>
+      <c r="L11" s="7">
+        <v>0</v>
+      </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="7"/>
@@ -1580,7 +1603,9 @@
       <c r="K12" s="7">
         <v>2.5</v>
       </c>
-      <c r="L12" s="8"/>
+      <c r="L12" s="7">
+        <v>2.5</v>
+      </c>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
       <c r="O12" s="7"/>
@@ -1620,7 +1645,9 @@
       <c r="K13" s="7">
         <v>2.5</v>
       </c>
-      <c r="L13" s="8"/>
+      <c r="L13" s="7">
+        <v>2.5</v>
+      </c>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="7"/>
@@ -1660,7 +1687,9 @@
       <c r="K14" s="7">
         <v>5</v>
       </c>
-      <c r="L14" s="8"/>
+      <c r="L14" s="7">
+        <v>5</v>
+      </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="7"/>
@@ -1700,7 +1729,9 @@
       <c r="K15" s="7">
         <v>5</v>
       </c>
-      <c r="L15" s="8"/>
+      <c r="L15" s="7">
+        <v>5</v>
+      </c>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
       <c r="O15" s="7"/>
@@ -1740,9 +1771,11 @@
         <v>18</v>
       </c>
       <c r="K16" s="7">
+        <v>18</v>
+      </c>
+      <c r="L16" s="7">
         <v>15</v>
       </c>
-      <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="7"/>
@@ -1782,7 +1815,9 @@
       <c r="K17" s="7">
         <v>20</v>
       </c>
-      <c r="L17" s="8"/>
+      <c r="L17" s="7">
+        <v>20</v>
+      </c>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="7"/>
@@ -1822,9 +1857,11 @@
         <v>18.5</v>
       </c>
       <c r="K18" s="7">
+        <v>18.5</v>
+      </c>
+      <c r="L18" s="7">
         <v>14.5</v>
       </c>
-      <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="7"/>
@@ -1864,9 +1901,11 @@
         <v>37</v>
       </c>
       <c r="K19" s="7">
+        <v>37</v>
+      </c>
+      <c r="L19" s="7">
         <v>35</v>
       </c>
-      <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
       <c r="O19" s="7"/>
@@ -1908,7 +1947,9 @@
       <c r="K20" s="7">
         <v>4</v>
       </c>
-      <c r="L20" s="8"/>
+      <c r="L20" s="7">
+        <v>4</v>
+      </c>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
       <c r="O20" s="7"/>
@@ -1948,9 +1989,11 @@
         <v>15</v>
       </c>
       <c r="K21" s="7">
+        <v>15</v>
+      </c>
+      <c r="L21" s="7">
         <v>9</v>
       </c>
-      <c r="L21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
       <c r="O21" s="7"/>
@@ -2032,7 +2075,7 @@
       <c r="B23" s="16"/>
       <c r="C23" s="17"/>
       <c r="D23" s="16">
-        <f t="shared" ref="D23:K23" si="0">SUM(D2:D21)</f>
+        <f t="shared" ref="D23:L23" si="0">SUM(D2:D21)</f>
         <v>190</v>
       </c>
       <c r="E23" s="16">
@@ -2061,9 +2104,12 @@
       </c>
       <c r="K23" s="16">
         <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+      <c r="L23" s="16">
+        <f t="shared" si="0"/>
         <v>125.5</v>
       </c>
-      <c r="L23" s="16"/>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
       <c r="O23" s="16"/>

</xml_diff>

<commit_message>
Oppdatert for martin og krisitna
</commit_message>
<xml_diff>
--- a/Sprint 4/SysUt14 Gr 2 Burn down chart - holdes oppdatert av SM.xlsx
+++ b/Sprint 4/SysUt14 Gr 2 Burn down chart - holdes oppdatert av SM.xlsx
@@ -432,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -487,9 +487,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -640,29 +637,35 @@
                 <c:pt idx="8">
                   <c:v>125.5</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>125.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>117</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50810240"/>
-        <c:axId val="51518464"/>
+        <c:axId val="91887488"/>
+        <c:axId val="91889024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50810240"/>
+        <c:axId val="91887488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51518464"/>
+        <c:crossAx val="91889024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51518464"/>
+        <c:axId val="91889024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -672,7 +675,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50810240"/>
+        <c:crossAx val="91887488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1068,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1174,12 +1177,16 @@
       <c r="L2" s="7">
         <v>0</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="M2" s="7">
+        <v>0</v>
+      </c>
+      <c r="N2" s="7">
+        <v>0</v>
+      </c>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
-      <c r="R2" s="23"/>
+      <c r="R2" s="22"/>
     </row>
     <row r="3" spans="1:18" ht="15.75">
       <c r="A3" s="5" t="s">
@@ -1218,12 +1225,16 @@
       <c r="L3" s="7">
         <v>0</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7">
+        <v>0</v>
+      </c>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
-      <c r="R3" s="23"/>
+      <c r="R3" s="22"/>
     </row>
     <row r="4" spans="1:18" ht="15.75">
       <c r="A4" s="5" t="s">
@@ -1262,12 +1273,16 @@
       <c r="L4" s="8">
         <v>0</v>
       </c>
-      <c r="M4" s="22"/>
-      <c r="N4" s="8"/>
+      <c r="M4" s="8">
+        <v>0</v>
+      </c>
+      <c r="N4" s="8">
+        <v>0</v>
+      </c>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="R4" s="23"/>
+      <c r="R4" s="22"/>
     </row>
     <row r="5" spans="1:18" ht="15.75">
       <c r="A5" s="5" t="s">
@@ -1306,12 +1321,16 @@
       <c r="L5" s="8">
         <v>1.5</v>
       </c>
-      <c r="M5" s="22"/>
-      <c r="N5" s="8"/>
+      <c r="M5" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="N5" s="8">
+        <v>1.5</v>
+      </c>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="R5" s="23"/>
+      <c r="R5" s="22"/>
     </row>
     <row r="6" spans="1:18" ht="15.75">
       <c r="A6" s="5"/>
@@ -1348,12 +1367,16 @@
       <c r="L6" s="8">
         <v>0.5</v>
       </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="8"/>
+      <c r="M6" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="N6" s="8">
+        <v>0.5</v>
+      </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="23"/>
+      <c r="R6" s="22"/>
     </row>
     <row r="7" spans="1:18" ht="15.75">
       <c r="A7" s="5"/>
@@ -1390,12 +1413,16 @@
       <c r="L7" s="8">
         <v>1</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
+      <c r="M7" s="8">
+        <v>1</v>
+      </c>
+      <c r="N7" s="8">
+        <v>1</v>
+      </c>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
-      <c r="R7" s="23"/>
+      <c r="R7" s="22"/>
     </row>
     <row r="8" spans="1:18" ht="15.75">
       <c r="A8" s="5" t="s">
@@ -1434,12 +1461,16 @@
       <c r="L8" s="8">
         <v>10</v>
       </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
+      <c r="M8" s="8">
+        <v>10</v>
+      </c>
+      <c r="N8" s="8">
+        <v>8</v>
+      </c>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
-      <c r="R8" s="23"/>
+      <c r="R8" s="22"/>
     </row>
     <row r="9" spans="1:18" ht="15.75">
       <c r="A9" s="5"/>
@@ -1476,12 +1507,16 @@
       <c r="L9" s="8">
         <v>0</v>
       </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
+      <c r="M9" s="8">
+        <v>0</v>
+      </c>
+      <c r="N9" s="8">
+        <v>0</v>
+      </c>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
-      <c r="R9" s="23"/>
+      <c r="R9" s="22"/>
     </row>
     <row r="10" spans="1:18" ht="15.75">
       <c r="A10" s="5" t="s">
@@ -1520,12 +1555,16 @@
       <c r="L10" s="7">
         <v>0</v>
       </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
+      <c r="M10" s="7">
+        <v>0</v>
+      </c>
+      <c r="N10" s="7">
+        <v>0</v>
+      </c>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
-      <c r="R10" s="23"/>
+      <c r="R10" s="22"/>
     </row>
     <row r="11" spans="1:18" ht="15.75">
       <c r="A11" s="5"/>
@@ -1562,12 +1601,16 @@
       <c r="L11" s="7">
         <v>0</v>
       </c>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
+      <c r="M11" s="7">
+        <v>0</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0</v>
+      </c>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
-      <c r="R11" s="23"/>
+      <c r="R11" s="22"/>
     </row>
     <row r="12" spans="1:18" ht="15.75">
       <c r="A12" s="5" t="s">
@@ -1606,12 +1649,16 @@
       <c r="L12" s="7">
         <v>2.5</v>
       </c>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
+      <c r="M12" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="N12" s="7">
+        <v>2.5</v>
+      </c>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
-      <c r="R12" s="23"/>
+      <c r="R12" s="22"/>
     </row>
     <row r="13" spans="1:18" ht="15.75">
       <c r="A13" s="5"/>
@@ -1648,12 +1695,16 @@
       <c r="L13" s="7">
         <v>2.5</v>
       </c>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
+      <c r="M13" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="N13" s="7">
+        <v>0.5</v>
+      </c>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
-      <c r="R13" s="23"/>
+      <c r="R13" s="22"/>
     </row>
     <row r="14" spans="1:18" ht="15.75">
       <c r="A14" s="5"/>
@@ -1690,12 +1741,16 @@
       <c r="L14" s="7">
         <v>5</v>
       </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
+      <c r="M14" s="7">
+        <v>5</v>
+      </c>
+      <c r="N14" s="7">
+        <v>5</v>
+      </c>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
-      <c r="R14" s="23"/>
+      <c r="R14" s="22"/>
     </row>
     <row r="15" spans="1:18" ht="15.75">
       <c r="A15" s="5"/>
@@ -1732,12 +1787,16 @@
       <c r="L15" s="7">
         <v>5</v>
       </c>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
+      <c r="M15" s="7">
+        <v>5</v>
+      </c>
+      <c r="N15" s="7">
+        <v>5</v>
+      </c>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
-      <c r="R15" s="23"/>
+      <c r="R15" s="22"/>
     </row>
     <row r="16" spans="1:18" ht="15.75">
       <c r="A16" s="5" t="s">
@@ -1776,12 +1835,16 @@
       <c r="L16" s="7">
         <v>15</v>
       </c>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
+      <c r="M16" s="7">
+        <v>15</v>
+      </c>
+      <c r="N16" s="7">
+        <v>15</v>
+      </c>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
-      <c r="R16" s="23"/>
+      <c r="R16" s="22"/>
     </row>
     <row r="17" spans="1:19" ht="15.75">
       <c r="A17" s="5"/>
@@ -1818,12 +1881,16 @@
       <c r="L17" s="7">
         <v>20</v>
       </c>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
+      <c r="M17" s="7">
+        <v>20</v>
+      </c>
+      <c r="N17" s="7">
+        <v>20</v>
+      </c>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
-      <c r="R17" s="23"/>
+      <c r="R17" s="22"/>
     </row>
     <row r="18" spans="1:19" ht="15.75">
       <c r="A18" s="5" t="s">
@@ -1862,12 +1929,16 @@
       <c r="L18" s="7">
         <v>14.5</v>
       </c>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
+      <c r="M18" s="7">
+        <v>14.5</v>
+      </c>
+      <c r="N18" s="7">
+        <v>10</v>
+      </c>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
-      <c r="R18" s="23"/>
+      <c r="R18" s="22"/>
     </row>
     <row r="19" spans="1:19" ht="15.75">
       <c r="A19" s="5" t="s">
@@ -1906,12 +1977,16 @@
       <c r="L19" s="7">
         <v>35</v>
       </c>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
+      <c r="M19" s="7">
+        <v>35</v>
+      </c>
+      <c r="N19" s="7">
+        <v>35</v>
+      </c>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
-      <c r="R19" s="23"/>
+      <c r="R19" s="22"/>
     </row>
     <row r="20" spans="1:19" ht="15.75">
       <c r="A20" s="5" t="s">
@@ -1950,12 +2025,16 @@
       <c r="L20" s="7">
         <v>4</v>
       </c>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
+      <c r="M20" s="7">
+        <v>4</v>
+      </c>
+      <c r="N20" s="7">
+        <v>4</v>
+      </c>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
-      <c r="R20" s="23"/>
+      <c r="R20" s="22"/>
     </row>
     <row r="21" spans="1:19" ht="15.75">
       <c r="A21" s="5" t="s">
@@ -1994,12 +2073,16 @@
       <c r="L21" s="7">
         <v>9</v>
       </c>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
+      <c r="M21" s="7">
+        <v>9</v>
+      </c>
+      <c r="N21" s="7">
+        <v>9</v>
+      </c>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
-      <c r="R21" s="23"/>
+      <c r="R21" s="22"/>
     </row>
     <row r="22" spans="1:19" ht="15.75">
       <c r="A22" s="10" t="s">
@@ -2075,7 +2158,7 @@
       <c r="B23" s="16"/>
       <c r="C23" s="17"/>
       <c r="D23" s="16">
-        <f t="shared" ref="D23:L23" si="0">SUM(D2:D21)</f>
+        <f t="shared" ref="D23:N23" si="0">SUM(D2:D21)</f>
         <v>190</v>
       </c>
       <c r="E23" s="16">
@@ -2110,8 +2193,14 @@
         <f t="shared" si="0"/>
         <v>125.5</v>
       </c>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
+      <c r="M23" s="16">
+        <f t="shared" si="0"/>
+        <v>125.5</v>
+      </c>
+      <c r="N23" s="16">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
       <c r="O23" s="16"/>
       <c r="P23" s="16"/>
       <c r="Q23" s="16"/>
@@ -2126,46 +2215,46 @@
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="24" t="s">
+      <c r="F24" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="24" t="s">
+      <c r="G24" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="H24" s="24" t="s">
+      <c r="H24" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="24" t="s">
+      <c r="I24" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="J24" s="24" t="s">
+      <c r="J24" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="K24" s="24" t="s">
+      <c r="K24" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="L24" s="24" t="s">
+      <c r="L24" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="M24" s="24" t="s">
+      <c r="M24" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="N24" s="24" t="s">
+      <c r="N24" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="O24" s="24" t="s">
+      <c r="O24" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="P24" s="24" t="s">
+      <c r="P24" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="Q24" s="24" t="s">
+      <c r="Q24" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="R24" s="25" t="s">
+      <c r="R24" s="24" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2174,28 +2263,28 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26" t="s">
+      <c r="F25" s="25"/>
+      <c r="G25" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26" t="s">
+      <c r="H25" s="25"/>
+      <c r="I25" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26" t="s">
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26" t="s">
+      <c r="M25" s="25"/>
+      <c r="N25" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26" t="s">
+      <c r="O25" s="25"/>
+      <c r="P25" s="25" t="s">
         <v>80</v>
       </c>
       <c r="Q25" s="1"/>

</xml_diff>

<commit_message>
Burn charts for torsdag 11.04
</commit_message>
<xml_diff>
--- a/Sprint 4/SysUt14 Gr 2 Burn down chart - holdes oppdatert av SM.xlsx
+++ b/Sprint 4/SysUt14 Gr 2 Burn down chart - holdes oppdatert av SM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -11,7 +11,7 @@
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -264,8 +264,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,12 +525,24 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="nb-NO"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -594,6 +606,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -644,41 +657,58 @@
                   <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>101</c:v>
+                  <c:v>89.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="74902528"/>
-        <c:axId val="74994432"/>
+        <c:smooth val="0"/>
+        <c:axId val="83831808"/>
+        <c:axId val="83833600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74902528"/>
+        <c:axId val="83831808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74994432"/>
+        <c:crossAx val="83833600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74994432"/>
+        <c:axId val="83833600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74902528"/>
+        <c:crossAx val="83831808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -686,6 +716,7 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -699,6 +730,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -862,6 +894,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -896,6 +929,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1071,14 +1105,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
@@ -1087,7 +1121,7 @@
     <col min="19" max="19" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75">
+    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -1143,7 +1177,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75">
+    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -1193,7 +1227,7 @@
       <c r="Q2" s="7"/>
       <c r="R2" s="22"/>
     </row>
-    <row r="3" spans="1:18" ht="15.75">
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -1243,7 +1277,7 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="22"/>
     </row>
-    <row r="4" spans="1:18" ht="15.75">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1293,7 +1327,7 @@
       <c r="Q4" s="7"/>
       <c r="R4" s="22"/>
     </row>
-    <row r="5" spans="1:18" ht="15.75">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>53</v>
       </c>
@@ -1337,13 +1371,13 @@
         <v>1.5</v>
       </c>
       <c r="O5" s="8">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="22"/>
     </row>
-    <row r="6" spans="1:18" ht="15.75">
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="21" t="s">
         <v>63</v>
@@ -1391,7 +1425,7 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="22"/>
     </row>
-    <row r="7" spans="1:18" ht="15.75">
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="21" t="s">
         <v>65</v>
@@ -1439,7 +1473,7 @@
       <c r="Q7" s="7"/>
       <c r="R7" s="22"/>
     </row>
-    <row r="8" spans="1:18" ht="15.75">
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1489,7 +1523,7 @@
       <c r="Q8" s="7"/>
       <c r="R8" s="22"/>
     </row>
-    <row r="9" spans="1:18" ht="15.75">
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="21" t="s">
         <v>39</v>
@@ -1537,7 +1571,7 @@
       <c r="Q9" s="7"/>
       <c r="R9" s="22"/>
     </row>
-    <row r="10" spans="1:18" ht="15.75">
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
@@ -1587,7 +1621,7 @@
       <c r="Q10" s="7"/>
       <c r="R10" s="22"/>
     </row>
-    <row r="11" spans="1:18" ht="15.75">
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="21" t="s">
         <v>32</v>
@@ -1635,7 +1669,7 @@
       <c r="Q11" s="7"/>
       <c r="R11" s="22"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75">
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>41</v>
       </c>
@@ -1685,7 +1719,7 @@
       <c r="Q12" s="7"/>
       <c r="R12" s="22"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75">
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="21" t="s">
         <v>43</v>
@@ -1733,7 +1767,7 @@
       <c r="Q13" s="7"/>
       <c r="R13" s="22"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75">
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="21" t="s">
         <v>44</v>
@@ -1781,7 +1815,7 @@
       <c r="Q14" s="7"/>
       <c r="R14" s="22"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75">
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="21" t="s">
         <v>44</v>
@@ -1829,7 +1863,7 @@
       <c r="Q15" s="7"/>
       <c r="R15" s="22"/>
     </row>
-    <row r="16" spans="1:18" ht="15.75">
+    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>45</v>
       </c>
@@ -1873,13 +1907,13 @@
         <v>7</v>
       </c>
       <c r="O16" s="7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="22"/>
     </row>
-    <row r="17" spans="1:19" ht="15.75">
+    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="21" t="s">
         <v>48</v>
@@ -1921,13 +1955,13 @@
         <v>20</v>
       </c>
       <c r="O17" s="7">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
       <c r="R17" s="22"/>
     </row>
-    <row r="18" spans="1:19" ht="15.75">
+    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>71</v>
       </c>
@@ -1977,7 +2011,7 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="22"/>
     </row>
-    <row r="19" spans="1:19" ht="15.75">
+    <row r="19" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>52</v>
       </c>
@@ -2027,7 +2061,7 @@
       <c r="Q19" s="7"/>
       <c r="R19" s="22"/>
     </row>
-    <row r="20" spans="1:19" ht="15.75">
+    <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>74</v>
       </c>
@@ -2077,7 +2111,7 @@
       <c r="Q20" s="7"/>
       <c r="R20" s="22"/>
     </row>
-    <row r="21" spans="1:19" ht="15.75">
+    <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>77</v>
       </c>
@@ -2127,7 +2161,7 @@
       <c r="Q21" s="7"/>
       <c r="R21" s="22"/>
     </row>
-    <row r="22" spans="1:19" ht="15.75">
+    <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>15</v>
       </c>
@@ -2194,7 +2228,7 @@
         <v>-7.1054273576010019E-15</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15.75">
+    <row r="23" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>16</v>
       </c>
@@ -2246,13 +2280,13 @@
       </c>
       <c r="O23" s="16">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>89.5</v>
       </c>
       <c r="P23" s="16"/>
       <c r="Q23" s="16"/>
       <c r="R23" s="18"/>
     </row>
-    <row r="24" spans="1:19" ht="15.75">
+    <row r="24" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>36</v>
       </c>
@@ -2304,7 +2338,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2347,24 +2381,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ferdigstilt for visning til kunde
Kommer nok noen endringer før vi leverer
</commit_message>
<xml_diff>
--- a/Sprint 4/SysUt14 Gr 2 Burn down chart - holdes oppdatert av SM.xlsx
+++ b/Sprint 4/SysUt14 Gr 2 Burn down chart - holdes oppdatert av SM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -11,7 +11,7 @@
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -264,8 +264,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -501,6 +501,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,24 +528,12 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="nb-NO"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -606,7 +597,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -659,56 +649,49 @@
                 <c:pt idx="11">
                   <c:v>89.5</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>62</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="83831808"/>
-        <c:axId val="83833600"/>
+        <c:axId val="113878528"/>
+        <c:axId val="113880064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83831808"/>
+        <c:axId val="113878528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83833600"/>
+        <c:crossAx val="113880064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83833600"/>
+        <c:axId val="113880064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
           <c:min val="0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83831808"/>
+        <c:crossAx val="113878528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -716,7 +699,6 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -730,7 +712,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -894,7 +875,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -929,7 +909,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1105,14 +1084,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="R16" sqref="D16:R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
@@ -1121,7 +1100,7 @@
     <col min="19" max="19" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="15.75">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -1177,7 +1156,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15.75">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -1223,11 +1202,17 @@
       <c r="O2" s="7">
         <v>0</v>
       </c>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="22"/>
+      <c r="P2" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>0</v>
+      </c>
+      <c r="R2" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15.75">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -1273,11 +1258,17 @@
       <c r="O3" s="7">
         <v>0</v>
       </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="22"/>
+      <c r="P3" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>0</v>
+      </c>
+      <c r="R3" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15.75">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1323,11 +1314,17 @@
       <c r="O4" s="8">
         <v>0</v>
       </c>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="22"/>
+      <c r="P4" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>0</v>
+      </c>
+      <c r="R4" s="26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15.75">
       <c r="A5" s="5" t="s">
         <v>53</v>
       </c>
@@ -1373,11 +1370,17 @@
       <c r="O5" s="8">
         <v>0</v>
       </c>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="22"/>
+      <c r="P5" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>0</v>
+      </c>
+      <c r="R5" s="26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15.75">
       <c r="A6" s="5"/>
       <c r="B6" s="21" t="s">
         <v>63</v>
@@ -1421,11 +1424,17 @@
       <c r="O6" s="8">
         <v>0.5</v>
       </c>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="22"/>
+      <c r="P6" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>0</v>
+      </c>
+      <c r="R6" s="26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15.75">
       <c r="A7" s="5"/>
       <c r="B7" s="21" t="s">
         <v>65</v>
@@ -1469,11 +1478,17 @@
       <c r="O7" s="8">
         <v>1</v>
       </c>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="22"/>
+      <c r="P7" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>0</v>
+      </c>
+      <c r="R7" s="26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15.75">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1519,11 +1534,17 @@
       <c r="O8" s="8">
         <v>7</v>
       </c>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="22"/>
+      <c r="P8" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>0</v>
+      </c>
+      <c r="R8" s="26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15.75">
       <c r="A9" s="5"/>
       <c r="B9" s="21" t="s">
         <v>39</v>
@@ -1567,11 +1588,17 @@
       <c r="O9" s="8">
         <v>0</v>
       </c>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="22"/>
+      <c r="P9" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>0</v>
+      </c>
+      <c r="R9" s="26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15.75">
       <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
@@ -1617,11 +1644,17 @@
       <c r="O10" s="7">
         <v>0</v>
       </c>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="22"/>
+      <c r="P10" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>0</v>
+      </c>
+      <c r="R10" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15.75">
       <c r="A11" s="5"/>
       <c r="B11" s="21" t="s">
         <v>32</v>
@@ -1665,11 +1698,17 @@
       <c r="O11" s="7">
         <v>0</v>
       </c>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="22"/>
+      <c r="P11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>0</v>
+      </c>
+      <c r="R11" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15.75">
       <c r="A12" s="5" t="s">
         <v>41</v>
       </c>
@@ -1715,11 +1754,17 @@
       <c r="O12" s="7">
         <v>2</v>
       </c>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="22"/>
+      <c r="P12" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>0</v>
+      </c>
+      <c r="R12" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15.75">
       <c r="A13" s="5"/>
       <c r="B13" s="21" t="s">
         <v>43</v>
@@ -1763,11 +1808,17 @@
       <c r="O13" s="7">
         <v>0</v>
       </c>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="22"/>
+      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>0</v>
+      </c>
+      <c r="R13" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15.75">
       <c r="A14" s="5"/>
       <c r="B14" s="21" t="s">
         <v>44</v>
@@ -1811,11 +1862,17 @@
       <c r="O14" s="7">
         <v>4</v>
       </c>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="22"/>
+      <c r="P14" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>0</v>
+      </c>
+      <c r="R14" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15.75">
       <c r="A15" s="5"/>
       <c r="B15" s="21" t="s">
         <v>44</v>
@@ -1859,11 +1916,17 @@
       <c r="O15" s="7">
         <v>4</v>
       </c>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="22"/>
+      <c r="P15" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>0</v>
+      </c>
+      <c r="R15" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="15.75">
       <c r="A16" s="5" t="s">
         <v>45</v>
       </c>
@@ -1909,11 +1972,17 @@
       <c r="O16" s="7">
         <v>4</v>
       </c>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="22"/>
+      <c r="P16" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>4</v>
+      </c>
+      <c r="R16" s="22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="15.75">
       <c r="A17" s="5"/>
       <c r="B17" s="21" t="s">
         <v>48</v>
@@ -1957,11 +2026,17 @@
       <c r="O17" s="7">
         <v>13</v>
       </c>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="22"/>
+      <c r="P17" s="7">
+        <v>13</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>13</v>
+      </c>
+      <c r="R17" s="22">
+        <v>13</v>
+      </c>
     </row>
-    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="15.75">
       <c r="A18" s="5" t="s">
         <v>71</v>
       </c>
@@ -2007,11 +2082,17 @@
       <c r="O18" s="7">
         <v>10</v>
       </c>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="22"/>
+      <c r="P18" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>10</v>
+      </c>
+      <c r="R18" s="22">
+        <v>10</v>
+      </c>
     </row>
-    <row r="19" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="15.75">
       <c r="A19" s="5" t="s">
         <v>52</v>
       </c>
@@ -2057,11 +2138,17 @@
       <c r="O19" s="7">
         <v>35</v>
       </c>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="22"/>
+      <c r="P19" s="7">
+        <v>35</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>35</v>
+      </c>
+      <c r="R19" s="22">
+        <v>35</v>
+      </c>
     </row>
-    <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="15.75">
       <c r="A20" s="5" t="s">
         <v>74</v>
       </c>
@@ -2107,11 +2194,17 @@
       <c r="O20" s="7">
         <v>4</v>
       </c>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="22"/>
+      <c r="P20" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>0</v>
+      </c>
+      <c r="R20" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="15.75">
       <c r="A21" s="5" t="s">
         <v>77</v>
       </c>
@@ -2157,11 +2250,17 @@
       <c r="O21" s="7">
         <v>5</v>
       </c>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="22"/>
+      <c r="P21" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>0</v>
+      </c>
+      <c r="R21" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="15.75">
       <c r="A22" s="10" t="s">
         <v>15</v>
       </c>
@@ -2228,14 +2327,14 @@
         <v>-7.1054273576010019E-15</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="15.75">
       <c r="A23" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="17"/>
       <c r="D23" s="16">
-        <f t="shared" ref="D23:O23" si="0">SUM(D2:D21)</f>
+        <f t="shared" ref="D23:R23" si="0">SUM(D2:D21)</f>
         <v>190</v>
       </c>
       <c r="E23" s="16">
@@ -2282,11 +2381,20 @@
         <f t="shared" si="0"/>
         <v>89.5</v>
       </c>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="18"/>
+      <c r="P23" s="16">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="Q23" s="16">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="R23" s="18">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
     </row>
-    <row r="24" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="15.75">
       <c r="A24" s="19" t="s">
         <v>36</v>
       </c>
@@ -2338,7 +2446,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2381,24 +2489,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>